<commit_message>
suite redy for grid execution
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ItemsModuleTest.xlsx
+++ b/resources/ExcelsheetData/ItemsModuleTest.xlsx
@@ -100,13 +100,13 @@
     <t>Taxonomy Name</t>
   </si>
   <si>
-    <t>Automation_Taxonomy</t>
-  </si>
-  <si>
     <t>Category Name</t>
   </si>
   <si>
-    <t>Automation_Category</t>
+    <t>AutomationTestTaxonomy</t>
+  </si>
+  <si>
+    <t>AutomationTestCat1</t>
   </si>
 </sst>
 </file>
@@ -804,7 +804,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:U1048576"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +834,7 @@
         <v>25</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
resolved exceptions and ready for grid execution
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ItemsModuleTest.xlsx
+++ b/resources/ExcelsheetData/ItemsModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="verifyDisplayOfNumRecordsChosen" sheetId="3" r:id="rId1"/>
@@ -14,13 +14,15 @@
     <sheet name="verifySearchInTaxonomyTree" sheetId="7" r:id="rId5"/>
     <sheet name="verifyRefreshInTaxonomyTree" sheetId="8" r:id="rId6"/>
     <sheet name="createNewCategory" sheetId="9" r:id="rId7"/>
+    <sheet name="verifyAddingAndClearingOfFilter" sheetId="10" r:id="rId8"/>
+    <sheet name="verifyGenralSearch" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -107,6 +109,48 @@
   </si>
   <si>
     <t>AutomationTestCat1</t>
+  </si>
+  <si>
+    <t>Test CaseId</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_013,TC_ITEMS_014</t>
+  </si>
+  <si>
+    <t>DropDownValues</t>
+  </si>
+  <si>
+    <t>Search Data</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_016</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>CIMM User</t>
+  </si>
+  <si>
+    <t>Subset</t>
+  </si>
+  <si>
+    <t>Static Pages</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_017</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_020</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_021</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_022</t>
   </si>
 </sst>
 </file>
@@ -169,13 +213,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,7 +849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -860,4 +906,116 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="7"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added surefire configuration xml attribute
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ItemsModuleTest.xlsx
+++ b/resources/ExcelsheetData/ItemsModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="verifyDisplayOfNumRecordsChosen" sheetId="3" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="createNewCategory" sheetId="9" r:id="rId7"/>
     <sheet name="verifyAddingAndClearingOfFilter" sheetId="10" r:id="rId8"/>
     <sheet name="verifyGenralSearch" sheetId="11" r:id="rId9"/>
+    <sheet name="validationOfTextboxes" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -117,12 +118,6 @@
     <t>TC_ITEMS_013,TC_ITEMS_014</t>
   </si>
   <si>
-    <t>DropDownValues</t>
-  </si>
-  <si>
-    <t>Search Data</t>
-  </si>
-  <si>
     <t>TC_ITEMS_016</t>
   </si>
   <si>
@@ -151,6 +146,99 @@
   </si>
   <si>
     <t>TC_ITEMS_022</t>
+  </si>
+  <si>
+    <t>Drop down value</t>
+  </si>
+  <si>
+    <t>Searchable data</t>
+  </si>
+  <si>
+    <t>AutomationTestSubset</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_028</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_029</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_030</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_031</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_032</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>Competitor Part Number</t>
+  </si>
+  <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>Data Source</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Quantity Available</t>
+  </si>
+  <si>
+    <t>List Price</t>
+  </si>
+  <si>
+    <t>Cost Price</t>
+  </si>
+  <si>
+    <t>Field Name</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_033</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_034</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_035</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_036</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_037</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_038</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_039</t>
+  </si>
+  <si>
+    <t>maximum number of characters that the textbox</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>AutomationTestPN1</t>
   </si>
 </sst>
 </file>
@@ -213,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -222,6 +310,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,6 +663,170 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
@@ -948,14 +1201,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD33"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -963,54 +1216,60 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="7"/>
+        <v>34</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="7"/>
     </row>

</xml_diff>

<commit_message>
downgrading surefire plugin to 2.18
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ItemsModuleTest.xlsx
+++ b/resources/ExcelsheetData/ItemsModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="verifyDisplayOfNumRecordsChosen" sheetId="3" r:id="rId1"/>
@@ -17,13 +17,16 @@
     <sheet name="verifyAddingAndClearingOfFilter" sheetId="10" r:id="rId8"/>
     <sheet name="verifyGenralSearch" sheetId="11" r:id="rId9"/>
     <sheet name="validationOfTextboxes" sheetId="12" r:id="rId10"/>
+    <sheet name="verifyRightNavigationBar" sheetId="13" r:id="rId11"/>
+    <sheet name="verifyAddingNewItem" sheetId="14" r:id="rId12"/>
+    <sheet name="verifyAddingNewItem_ES" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="90">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -239,6 +242,60 @@
   </si>
   <si>
     <t>AutomationTestPN1</t>
+  </si>
+  <si>
+    <t>Mandotory Fields</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_023</t>
+  </si>
+  <si>
+    <t>Attributes in Right panel</t>
+  </si>
+  <si>
+    <t>Manufacturer,Part Number,Brand</t>
+  </si>
+  <si>
+    <t>MPN,Part No.,List Price,Cost Price,User Rating,Hits,Popularity</t>
+  </si>
+  <si>
+    <t>Item saved Successfully</t>
+  </si>
+  <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>ManufactureName</t>
+  </si>
+  <si>
+    <t>PartNumber Field</t>
+  </si>
+  <si>
+    <t>BrandName</t>
+  </si>
+  <si>
+    <t>SuccessMessage</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_024</t>
+  </si>
+  <si>
+    <t>AutomationTestManufacturer</t>
+  </si>
+  <si>
+    <t>AutomationTestBrand</t>
+  </si>
+  <si>
+    <t>AutomationTestPN</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_025</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_026</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_027</t>
   </si>
 </sst>
 </file>
@@ -827,6 +884,190 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
@@ -1200,7 +1441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Item module- completed till 50 test case
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ItemsModuleTest.xlsx
+++ b/resources/ExcelsheetData/ItemsModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="6" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="12" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="verifyDisplayOfNumRecordsChosen" sheetId="3" r:id="rId1"/>
@@ -21,14 +21,17 @@
     <sheet name="validationOfTextboxes" sheetId="12" r:id="rId12"/>
     <sheet name="verifyRightNavigationBar" sheetId="13" r:id="rId13"/>
     <sheet name="verifyAddingNewItem" sheetId="14" r:id="rId14"/>
-    <sheet name="verifyAddingNewItem_ES" sheetId="15" r:id="rId15"/>
+    <sheet name="addNewWorkbook" sheetId="18" r:id="rId15"/>
+    <sheet name="addItemsToWorkbook" sheetId="19" r:id="rId16"/>
+    <sheet name="MessageofAddItemsToWorkbook" sheetId="20" r:id="rId17"/>
+    <sheet name="verifyAddingNewItem_ES" sheetId="15" r:id="rId18"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="122">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -325,6 +328,75 @@
   </si>
   <si>
     <t>Print</t>
+  </si>
+  <si>
+    <t>Select Manufacturer Name</t>
+  </si>
+  <si>
+    <t>Part Number Required</t>
+  </si>
+  <si>
+    <t>Select Brand</t>
+  </si>
+  <si>
+    <t>TestCase Name</t>
+  </si>
+  <si>
+    <t>WorkBookName</t>
+  </si>
+  <si>
+    <t>WorkBook SuccessMessage</t>
+  </si>
+  <si>
+    <t>WorkBookRemove Message</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_45</t>
+  </si>
+  <si>
+    <t>AutomationTestWorkBook</t>
+  </si>
+  <si>
+    <t>removed Successfully</t>
+  </si>
+  <si>
+    <t>WorkBook saved Successfully</t>
+  </si>
+  <si>
+    <t>Rename Error Message</t>
+  </si>
+  <si>
+    <t>WorkBook Name already exists</t>
+  </si>
+  <si>
+    <t>TestCasesId</t>
+  </si>
+  <si>
+    <t>workBookSuccesMsg</t>
+  </si>
+  <si>
+    <t>noOfItemsToBeSelect</t>
+  </si>
+  <si>
+    <t>additemWorkbooksuccessmsg</t>
+  </si>
+  <si>
+    <t>workbookRemovemsg</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_47</t>
+  </si>
+  <si>
+    <t>AlertMessage</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_49</t>
+  </si>
+  <si>
+    <t>Checking this will add all Items into workbook when a chosen workbook is triggered</t>
   </si>
 </sst>
 </file>
@@ -387,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -406,6 +478,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,7 +835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1155,10 +1228,162 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,76 +1392,85 @@
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="7" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Items module has been completed
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/ItemsModuleTest.xlsx
+++ b/resources/ExcelsheetData/ItemsModuleTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="58" activeTab="63"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="verifyDisplayOfNumRecordsChosen" sheetId="3" r:id="rId1"/>
@@ -18,78 +18,93 @@
     <sheet name="verifyItemStatusDropdown" sheetId="16" r:id="rId9"/>
     <sheet name="verifyCheckboxes" sheetId="17" r:id="rId10"/>
     <sheet name="verifyGenralSearch" sheetId="11" r:id="rId11"/>
-    <sheet name="validationOfTextboxes" sheetId="12" r:id="rId12"/>
-    <sheet name="verifyRightNavigationBar" sheetId="13" r:id="rId13"/>
-    <sheet name="verifyAddingNewItem" sheetId="14" r:id="rId14"/>
-    <sheet name="addNewWorkbook" sheetId="18" r:id="rId15"/>
-    <sheet name="addItemsToWorkbook" sheetId="19" r:id="rId16"/>
-    <sheet name="MessageofAddItemsToWorkbook" sheetId="20" r:id="rId17"/>
-    <sheet name="verificationOfRightPanel" sheetId="21" r:id="rId18"/>
-    <sheet name="verifySearchFnEditItem" sheetId="22" r:id="rId19"/>
-    <sheet name="verifyNextPreviousEditItem" sheetId="23" r:id="rId20"/>
-    <sheet name="verifyGeneralInfoTab" sheetId="24" r:id="rId21"/>
-    <sheet name="verifyItemUpdateFunctionality" sheetId="25" r:id="rId22"/>
-    <sheet name="verifyResetFunctionality" sheetId="26" r:id="rId23"/>
-    <sheet name="verifyHistory" sheetId="27" r:id="rId24"/>
-    <sheet name="verifyDescriptionTab" sheetId="28" r:id="rId25"/>
-    <sheet name="verificationOfDescLang" sheetId="32" r:id="rId26"/>
-    <sheet name="verifyHistoryLinkInDesc" sheetId="33" r:id="rId27"/>
-    <sheet name="verificationOFProductsTab" sheetId="34" r:id="rId28"/>
-    <sheet name="verifyProductSave" sheetId="35" r:id="rId29"/>
-    <sheet name="verifyTinyMceEditorDisplay" sheetId="29" r:id="rId30"/>
-    <sheet name="verifyKeywordsTab" sheetId="36" r:id="rId31"/>
-    <sheet name="verifyKeywordsTabMeta" sheetId="37" r:id="rId32"/>
-    <sheet name="verifyKeywordsTabCustom" sheetId="38" r:id="rId33"/>
-    <sheet name="verifyKeywordsUpdate" sheetId="39" r:id="rId34"/>
-    <sheet name="verifyKeywordsHistory" sheetId="40" r:id="rId35"/>
-    <sheet name="addDocumenttoItems" sheetId="41" r:id="rId36"/>
-    <sheet name="verifyAddNewDocument" sheetId="42" r:id="rId37"/>
-    <sheet name="addDocumentURLtoItems" sheetId="43" r:id="rId38"/>
-    <sheet name="addDocumentURL_ES" sheetId="46" r:id="rId39"/>
-    <sheet name="addNewItemDocDescription" sheetId="47" r:id="rId40"/>
-    <sheet name="validateDocCategoryName" sheetId="48" r:id="rId41"/>
-    <sheet name="validateDocCategoryDescription" sheetId="49" r:id="rId42"/>
-    <sheet name="verifyDocDescriptionHistory" sheetId="50" r:id="rId43"/>
-    <sheet name="verifyItemVideosTab" sheetId="51" r:id="rId44"/>
-    <sheet name="verifyAddNewVideoWindow" sheetId="52" r:id="rId45"/>
-    <sheet name="verifyAddNewVideo" sheetId="53" r:id="rId46"/>
-    <sheet name="verifyAddNewVideo_ES" sheetId="54" r:id="rId47"/>
-    <sheet name="verifyLinkedItems" sheetId="55" r:id="rId48"/>
-    <sheet name="verifyLinkedItemsFields" sheetId="56" r:id="rId49"/>
-    <sheet name="verifyAssignedLinkedItems" sheetId="57" r:id="rId50"/>
-    <sheet name="verifyAvailableLinkedItems" sheetId="58" r:id="rId51"/>
-    <sheet name="verifyListItemLinkType" sheetId="59" r:id="rId52"/>
-    <sheet name="updateItemLinkType" sheetId="60" r:id="rId53"/>
-    <sheet name="verifyAttributesPage" sheetId="61" r:id="rId54"/>
-    <sheet name="verifySaveAttribute" sheetId="62" r:id="rId55"/>
-    <sheet name="verifyCancelAttribute" sheetId="63" r:id="rId56"/>
-    <sheet name="verifyCustomPricesTab" sheetId="64" r:id="rId57"/>
-    <sheet name="verifyCustomPriceCheckBox" sheetId="65" r:id="rId58"/>
-    <sheet name="verifyCustomPriceTextFields" sheetId="66" r:id="rId59"/>
-    <sheet name="validateCustomPriceTextFields" sheetId="67" r:id="rId60"/>
-    <sheet name="verifySubsetStatus" sheetId="68" r:id="rId61"/>
-    <sheet name="updateCustomPrice" sheetId="69" r:id="rId62"/>
-    <sheet name="verifyCPHistory" sheetId="70" r:id="rId63"/>
-    <sheet name="verifyCategoryHistory" sheetId="71" r:id="rId64"/>
-    <sheet name="verifyCustomFieldsTab" sheetId="72" r:id="rId65"/>
-    <sheet name="verifyCFSimpleData" sheetId="73" r:id="rId66"/>
-    <sheet name="verifyCPTab" sheetId="74" r:id="rId67"/>
-    <sheet name="verifyAddNewCPNPage" sheetId="75" r:id="rId68"/>
-    <sheet name="verifyCustomerDropDown" sheetId="76" r:id="rId69"/>
-    <sheet name="verifyCPNReset" sheetId="77" r:id="rId70"/>
-    <sheet name="verifyWarehouse" sheetId="78" r:id="rId71"/>
-    <sheet name="updateDocCationToItems" sheetId="44" r:id="rId72"/>
-    <sheet name="verificationOfCancel" sheetId="45" r:id="rId73"/>
-    <sheet name="verificationOfEditItemPage" sheetId="30" r:id="rId74"/>
-    <sheet name="verificationOfUpdatingDesc" sheetId="31" r:id="rId75"/>
-    <sheet name="verifyAddingNewItem_ES" sheetId="15" r:id="rId76"/>
+    <sheet name="verifyCFTable" sheetId="94" r:id="rId12"/>
+    <sheet name="validationOfTextboxes" sheetId="12" r:id="rId13"/>
+    <sheet name="verifyRightNavigationBar" sheetId="13" r:id="rId14"/>
+    <sheet name="verifyAddingNewItem" sheetId="14" r:id="rId15"/>
+    <sheet name="addNewWorkbook" sheetId="18" r:id="rId16"/>
+    <sheet name="addItemsToWorkbook" sheetId="19" r:id="rId17"/>
+    <sheet name="MessageofAddItemsToWorkbook" sheetId="20" r:id="rId18"/>
+    <sheet name="verificationOfRightPanel" sheetId="21" r:id="rId19"/>
+    <sheet name="verifySearchFnEditItem" sheetId="22" r:id="rId20"/>
+    <sheet name="verifyNextPreviousEditItem" sheetId="23" r:id="rId21"/>
+    <sheet name="verifyGeneralInfoTab" sheetId="24" r:id="rId22"/>
+    <sheet name="verifyItemUpdateFunctionality" sheetId="25" r:id="rId23"/>
+    <sheet name="verifyResetFunctionality" sheetId="26" r:id="rId24"/>
+    <sheet name="verifyHistory" sheetId="27" r:id="rId25"/>
+    <sheet name="verifyDescriptionTab" sheetId="28" r:id="rId26"/>
+    <sheet name="verificationOfDescLang" sheetId="32" r:id="rId27"/>
+    <sheet name="verifyHistoryLinkInDesc" sheetId="33" r:id="rId28"/>
+    <sheet name="verificationOFProductsTab" sheetId="34" r:id="rId29"/>
+    <sheet name="verifyProductSave" sheetId="35" r:id="rId30"/>
+    <sheet name="verifyTinyMceEditorDisplay" sheetId="29" r:id="rId31"/>
+    <sheet name="verifyKeywordsTab" sheetId="36" r:id="rId32"/>
+    <sheet name="verifyKeywordsTabMeta" sheetId="37" r:id="rId33"/>
+    <sheet name="verifyKeywordsTabCustom" sheetId="38" r:id="rId34"/>
+    <sheet name="verifyKeywordsUpdate" sheetId="39" r:id="rId35"/>
+    <sheet name="verifyKeywordsHistory" sheetId="40" r:id="rId36"/>
+    <sheet name="addDocumenttoItems" sheetId="41" r:id="rId37"/>
+    <sheet name="verifyAddNewDocument" sheetId="42" r:id="rId38"/>
+    <sheet name="addDocumentURLtoItems" sheetId="43" r:id="rId39"/>
+    <sheet name="addDocumentURL_ES" sheetId="46" r:id="rId40"/>
+    <sheet name="addNewItemDocDescription" sheetId="47" r:id="rId41"/>
+    <sheet name="validateDocCategoryName" sheetId="48" r:id="rId42"/>
+    <sheet name="validateDocCategoryDescription" sheetId="49" r:id="rId43"/>
+    <sheet name="verifyDocDescriptionHistory" sheetId="50" r:id="rId44"/>
+    <sheet name="verifyItemVideosTab" sheetId="51" r:id="rId45"/>
+    <sheet name="verifyAddNewVideoWindow" sheetId="52" r:id="rId46"/>
+    <sheet name="verifyAddNewVideo" sheetId="53" r:id="rId47"/>
+    <sheet name="verifyAddNewVideo_ES" sheetId="54" r:id="rId48"/>
+    <sheet name="verifyLinkedItems" sheetId="55" r:id="rId49"/>
+    <sheet name="verifyLinkedItemsFields" sheetId="56" r:id="rId50"/>
+    <sheet name="verifyAssignedLinkedItems" sheetId="57" r:id="rId51"/>
+    <sheet name="verifyAvailableLinkedItems" sheetId="58" r:id="rId52"/>
+    <sheet name="verifyListItemLinkType" sheetId="59" r:id="rId53"/>
+    <sheet name="updateItemLinkType" sheetId="60" r:id="rId54"/>
+    <sheet name="verifyAttributesPage" sheetId="61" r:id="rId55"/>
+    <sheet name="verifySaveAttribute" sheetId="62" r:id="rId56"/>
+    <sheet name="verifyCancelAttribute" sheetId="63" r:id="rId57"/>
+    <sheet name="verifyCustomPricesTab" sheetId="64" r:id="rId58"/>
+    <sheet name="verifyCustomPriceCheckBox" sheetId="65" r:id="rId59"/>
+    <sheet name="verifyCustomPriceTextFields" sheetId="66" r:id="rId60"/>
+    <sheet name="validateCustomPriceTextFields" sheetId="67" r:id="rId61"/>
+    <sheet name="verifySubsetStatus" sheetId="68" r:id="rId62"/>
+    <sheet name="updateCustomPrice" sheetId="69" r:id="rId63"/>
+    <sheet name="verifyCPHistory" sheetId="70" r:id="rId64"/>
+    <sheet name="verifyCategoryHistory" sheetId="71" r:id="rId65"/>
+    <sheet name="verifyCustomFieldsTab" sheetId="72" r:id="rId66"/>
+    <sheet name="verifyCFSimpleData" sheetId="73" r:id="rId67"/>
+    <sheet name="verifyCPTab" sheetId="74" r:id="rId68"/>
+    <sheet name="verifyAddNewCPNPage" sheetId="75" r:id="rId69"/>
+    <sheet name="verifyCustomerDropDown" sheetId="76" r:id="rId70"/>
+    <sheet name="verifyCPNReset" sheetId="77" r:id="rId71"/>
+    <sheet name="verifyWarehouse" sheetId="78" r:id="rId72"/>
+    <sheet name="verifyWarehouseSearch" sheetId="80" r:id="rId73"/>
+    <sheet name="verifyWarehouseSearch_ES" sheetId="81" r:id="rId74"/>
+    <sheet name="verifySaveWarehouse" sheetId="82" r:id="rId75"/>
+    <sheet name="verifySaveMultiWarehouses" sheetId="83" r:id="rId76"/>
+    <sheet name="verifySaveAllWarehouses" sheetId="85" r:id="rId77"/>
+    <sheet name="verifyRemoveMultiWarehouses" sheetId="86" r:id="rId78"/>
+    <sheet name="verifyRemoveAllWarehouses" sheetId="87" r:id="rId79"/>
+    <sheet name="verifyHistoryWarehouses" sheetId="88" r:id="rId80"/>
+    <sheet name="verifyCopyOfItem" sheetId="89" r:id="rId81"/>
+    <sheet name="validateInputFields" sheetId="90" r:id="rId82"/>
+    <sheet name="verificationOfInputFields" sheetId="91" r:id="rId83"/>
+    <sheet name="verifyResetCopyItem" sheetId="92" r:id="rId84"/>
+    <sheet name="verifySaveCopyItem" sheetId="93" r:id="rId85"/>
+    <sheet name="verifyRemoveWarehouse" sheetId="84" r:id="rId86"/>
+    <sheet name="updateDocCationToItems" sheetId="44" r:id="rId87"/>
+    <sheet name="verificationOfCancel" sheetId="45" r:id="rId88"/>
+    <sheet name="verificationOfEditItemPage" sheetId="30" r:id="rId89"/>
+    <sheet name="verificationOfUpdatingDesc" sheetId="31" r:id="rId90"/>
+    <sheet name="verifyAddingNewItem_ES" sheetId="15" r:id="rId91"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="388">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -565,9 +580,6 @@
     <t>History will be opened in new tab/window</t>
   </si>
   <si>
-    <t>CIMM2 -Item General Info Changes History</t>
-  </si>
-  <si>
     <t>TC_ITEMS_62</t>
   </si>
   <si>
@@ -808,9 +820,6 @@
     <t>CIMM2 -Item Document History</t>
   </si>
   <si>
-    <t>CIMM2 -Item Keywords History</t>
-  </si>
-  <si>
     <t>TC_ITEMS_98</t>
   </si>
   <si>
@@ -1087,9 +1096,6 @@
     <t>TC_ITEMS_141</t>
   </si>
   <si>
-    <t>CIMM2 -Item Categorization History</t>
-  </si>
-  <si>
     <t>Categorization HistoryTitle</t>
   </si>
   <si>
@@ -1121,6 +1127,147 @@
   </si>
   <si>
     <t>TC_ITEMS_158</t>
+  </si>
+  <si>
+    <t>Part number</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_159</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_160</t>
+  </si>
+  <si>
+    <t>warehouseName</t>
+  </si>
+  <si>
+    <t>AutomationTestWarehouse</t>
+  </si>
+  <si>
+    <t>AutomationTestInvalidName</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_161</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_162</t>
+  </si>
+  <si>
+    <t>Warehouse Item updated Successfully</t>
+  </si>
+  <si>
+    <t>warehouse Success Message</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_163</t>
+  </si>
+  <si>
+    <t>Warehouse Item Removed Successfully</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_165</t>
+  </si>
+  <si>
+    <t>noOfWareHosesToBeSelect</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_164</t>
+  </si>
+  <si>
+    <t>no of Warehouses to be select</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_166</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_167</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_168</t>
+  </si>
+  <si>
+    <t>Alert Message</t>
+  </si>
+  <si>
+    <t>Page Title</t>
+  </si>
+  <si>
+    <t>CIMM2Touch - Warehouse Item Histroy</t>
+  </si>
+  <si>
+    <t>CIMM2Touch -Item General Info Changes History</t>
+  </si>
+  <si>
+    <t>CIMM2Touch -Item Keywords History</t>
+  </si>
+  <si>
+    <t>CIMM2Touch -Item Categorization History</t>
+  </si>
+  <si>
+    <t>Input Fields Name</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_169</t>
+  </si>
+  <si>
+    <t>New Part Number,No.of Copies,Item Status,Display Online</t>
+  </si>
+  <si>
+    <t>Item Info Tabs</t>
+  </si>
+  <si>
+    <t>Item General Info,Item Descriptions,Item Keywords,Item Documents,Item Images,Item Linked Items,Item Attributes,Item Custom Prices,Item Categorization,Custom Fields</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>partNumber</t>
+  </si>
+  <si>
+    <t>noOfCopies</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_170</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_171</t>
+  </si>
+  <si>
+    <t>AutomationTestPNCopy</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_172</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_173</t>
+  </si>
+  <si>
+    <t>exp Error Message</t>
+  </si>
+  <si>
+    <t>Number Of Copies Required</t>
+  </si>
+  <si>
+    <t>Exp Succes Message</t>
+  </si>
+  <si>
+    <t>Save Successfully</t>
+  </si>
+  <si>
+    <t>TC_ITEMS_175</t>
+  </si>
+  <si>
+    <t>Taxonomy</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1226,6 +1373,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1634,7 +1792,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,7 +1854,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1706,7 +1864,9 @@
       <c r="B6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>345</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1715,6 +1875,41 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:AA1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -1878,7 +2073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1920,7 +2115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1975,7 +2170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2031,7 +2226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2087,7 +2282,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2122,7 +2317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -2216,41 +2411,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
@@ -2319,6 +2479,41 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -2349,7 +2544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2405,7 +2600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2481,7 +2676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2544,12 +2739,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2557,7 +2752,7 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2585,15 +2780,15 @@
         <v>157</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>365</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2616,26 +2811,26 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -2658,37 +2853,37 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2712,15 +2907,15 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
@@ -2729,15 +2924,15 @@
         <v>157</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2760,26 +2955,75 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>174</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>173</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2804,87 +3048,38 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2907,26 +3102,26 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="300.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="300.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>163</v>
-      </c>
       <c r="C2" s="13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2945,23 +3140,23 @@
         <v>77</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2984,26 +3179,26 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3026,26 +3221,26 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>186</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3068,26 +3263,26 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -3112,38 +3307,38 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>157</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>366</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3161,52 +3356,52 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3229,26 +3424,26 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -3267,16 +3462,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>202</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>81</v>
@@ -3284,27 +3479,76 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -3324,63 +3568,63 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>207</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>208</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>70</v>
@@ -3388,67 +3632,18 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>223</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -3467,44 +3662,44 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>201</v>
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="E1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3521,32 +3716,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>201</v>
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>233</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3563,32 +3758,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>201</v>
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>234</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -3606,21 +3801,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>201</v>
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>154</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
@@ -3629,15 +3824,15 @@
         <v>157</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3653,26 +3848,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>201</v>
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>238</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3688,26 +3883,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>201</v>
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>238</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3730,47 +3925,47 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>242</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>244</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>81</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -3794,19 +3989,19 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>242</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>243</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>244</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>81</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>154</v>
@@ -3814,33 +4009,33 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>247</v>
-      </c>
       <c r="G2" s="15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -3859,57 +4054,15 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3974,6 +4127,48 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3996,24 +4191,24 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>257</v>
-      </c>
       <c r="F1" s="14" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
@@ -4022,21 +4217,21 @@
         <v>85</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2" t="s">
         <v>259</v>
       </c>
-      <c r="F2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -4056,29 +4251,29 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -4098,29 +4293,29 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>266</v>
-      </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -4143,47 +4338,47 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>259</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4204,24 +4399,24 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>273</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>275</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>26</v>
@@ -4232,7 +4427,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -4254,41 +4449,41 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>280</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>279</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>26</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4309,24 +4504,24 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>26</v>
@@ -4337,7 +4532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -4357,29 +4552,29 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4398,47 +4593,12 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
@@ -4451,10 +4611,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4464,9 +4624,10 @@
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4482,8 +4643,11 @@
       <c r="E1" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="22" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -4499,6 +4663,9 @@
       <c r="E2" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="F2" s="23" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4506,6 +4673,41 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -4527,211 +4729,211 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="D1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>291</v>
-      </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>116</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>69</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>317</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>315</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -4752,24 +4954,24 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>318</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>320</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>42</v>
@@ -4777,13 +4979,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>42</v>
@@ -4794,7 +4996,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4815,24 +5017,24 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>325</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>327</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>42</v>
@@ -4843,7 +5045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -4864,18 +5066,18 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
@@ -4884,19 +5086,19 @@
         <v>157</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>330</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -4905,7 +5107,7 @@
     <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -4913,18 +5115,18 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
@@ -4933,15 +5135,15 @@
         <v>157</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>332</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>367</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4960,23 +5162,23 @@
         <v>89</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>331</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -4999,26 +5201,26 @@
         <v>48</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>337</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -5042,18 +5244,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>338</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>335</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -5077,52 +5279,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>342</v>
+        <v>336</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -5198,6 +5358,48 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD36"/>
     </sheetView>
   </sheetViews>
@@ -5216,8 +5418,85 @@
         <v>134</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>340</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -5227,32 +5506,783 @@
         <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>346</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>355</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>364</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="157.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="9" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="25" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>379</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>352</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5267,16 +6297,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>202</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>81</v>
@@ -5287,30 +6317,30 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="F2" t="s">
         <v>210</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="F2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -5330,16 +6360,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>202</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>81</v>
@@ -5350,30 +6380,30 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="F2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>210</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -5397,7 +6427,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>120</v>
@@ -5408,7 +6438,51 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="117.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5428,7 +6502,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -5522,83 +6596,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="117.42578125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="56.28515625" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="9"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>